<commit_message>
prompts for company info,etc.
</commit_message>
<xml_diff>
--- a/Financial_Statement.xlsx
+++ b/Financial_Statement.xlsx
@@ -466,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,10 +474,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="35" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -487,45 +490,72 @@
         </is>
       </c>
       <c r="B1" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="F1" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="G1" s="1" t="n">
         <v>2024</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>2025</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Revenue</t>
+          <t>Sales</t>
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>627361</v>
+        <v>2572322</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>531879</v>
+        <v>2479559</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>330260</v>
+        <v>2226089</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>2500370</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>2477135</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>2576903</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total Revenue</t>
-        </is>
-      </c>
-      <c r="B3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>0</v>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>2572322</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>2479559</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>2226089</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>2500370</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>2477135</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>2576903</v>
       </c>
     </row>
     <row r="4">
@@ -534,420 +564,654 @@
           <t>Cost of Goods Sold</t>
         </is>
       </c>
-      <c r="B4" s="3" t="n">
-        <v>141138</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>174592</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>39125</v>
+      <c r="B4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Gross Profit</t>
+          <t>Cost of sales</t>
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>486223</v>
+        <v>740359</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>357287</v>
+        <v>667168</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>291135</v>
+        <v>617403</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>734227</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>839960</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>874396</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>Gross Profit Margin (%)</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4" t="n">
-        <v>0</v>
+          <t>Total Cost of Goods Sold</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>740359</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>667168</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>617403</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>734227</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>839960</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>874396</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>Expenses</t>
-        </is>
-      </c>
-      <c r="B7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4" t="n">
-        <v>0</v>
+          <t>Gross (loss) profit</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>1831963</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>1812391</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>1608686</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>1766143</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>1637175</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>1702507</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Advertising</t>
-        </is>
-      </c>
-      <c r="B8" s="3" t="n">
-        <v>4679</v>
-      </c>
-      <c r="C8" s="3" t="n">
-        <v>2874</v>
-      </c>
-      <c r="D8" s="3" t="n">
-        <v>889</v>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Amortization</t>
-        </is>
-      </c>
-      <c r="B9" s="4" t="n">
-        <v>0</v>
+          <t>Advertising and promotion</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>3872</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>45949</v>
+        <v>3104</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>30020</v>
+        <v>599</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>500</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>3349</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Charitable donations</t>
-        </is>
-      </c>
-      <c r="B10" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="4" t="n">
-        <v>0</v>
+          <t>Commissions</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>205330</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>187678</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>4000</v>
+        <v>148355</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>157247</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>160671</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>197579</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Insurance</t>
+          <t>Insurance</t>
         </is>
       </c>
       <c r="B11" s="3" t="n">
-        <v>2788</v>
+        <v>36010</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>2687</v>
+        <v>27938</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>1568</v>
+        <v>49567</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>47967</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>51854</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>36126</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Interest expense</t>
+          <t>Interest and bank charges</t>
         </is>
       </c>
       <c r="B12" s="3" t="n">
-        <v>18300</v>
+        <v>15940</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>16776</v>
+        <v>21295</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>4093</v>
+        <v>18737</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>9638</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>15825</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <v>37763</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Meals</t>
+          <t>Meals and entertainment</t>
         </is>
       </c>
       <c r="B13" s="3" t="n">
-        <v>4657</v>
+        <v>2037</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>5830</v>
+        <v>189</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>4619</v>
+        <v>2381</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>2481</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <v>3301</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Office expense</t>
+          <t>Office</t>
         </is>
       </c>
       <c r="B14" s="3" t="n">
-        <v>22184</v>
+        <v>15242</v>
       </c>
       <c r="C14" s="3" t="n">
-        <v>36197</v>
+        <v>29336</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>37638</v>
+        <v>31872</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>12198</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>9513</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <v>14859</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Professional fees</t>
+          <t>Professional fees</t>
         </is>
       </c>
       <c r="B15" s="3" t="n">
-        <v>2800</v>
+        <v>38374</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>2200</v>
+        <v>35927</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>2500</v>
+        <v>11462</v>
+      </c>
+      <c r="E15" s="3" t="n">
+        <v>15466</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>6958</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <v>6031</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Rent</t>
+          <t>Promotions and discounts</t>
         </is>
       </c>
       <c r="B16" s="3" t="n">
-        <v>14866</v>
+        <v>2329</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>16175</v>
+        <v>9468</v>
       </c>
       <c r="D16" s="3" t="n">
-        <v>10400</v>
+        <v>2676</v>
+      </c>
+      <c r="E16" s="3" t="n">
+        <v>293</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>1307</v>
+      </c>
+      <c r="G16" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Telephone</t>
+          <t>Publications and subscriptions</t>
         </is>
       </c>
       <c r="B17" s="3" t="n">
-        <v>4639</v>
+        <v>12576</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>4876</v>
+        <v>7885</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>1390</v>
+        <v>10106</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>22053</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>15220</v>
+      </c>
+      <c r="G17" s="3" t="n">
+        <v>6146</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Travel</t>
+          <t>Rental</t>
         </is>
       </c>
       <c r="B18" s="3" t="n">
-        <v>8910</v>
+        <v>154964</v>
       </c>
       <c r="C18" s="3" t="n">
-        <v>2876</v>
+        <v>157500</v>
       </c>
       <c r="D18" s="3" t="n">
-        <v>121</v>
+        <v>160416</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>157500</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>157689</v>
+      </c>
+      <c r="G18" s="3" t="n">
+        <v>157500</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Wages &amp; benefits</t>
+          <t>Repairs and maintenance</t>
         </is>
       </c>
       <c r="B19" s="3" t="n">
-        <v>23523</v>
+        <v>49442</v>
       </c>
       <c r="C19" s="3" t="n">
-        <v>15311</v>
-      </c>
-      <c r="D19" s="4" t="n">
-        <v>0</v>
+        <v>23714</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>16966</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>11120</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>16258</v>
+      </c>
+      <c r="G19" s="3" t="n">
+        <v>18372</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Other Expenses</t>
-        </is>
-      </c>
-      <c r="B20" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="4" t="n">
-        <v>0</v>
+          <t>Salaries, wages and benefits</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="n">
+        <v>860192</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>865797</v>
       </c>
       <c r="D20" s="3" t="n">
-        <v>4761</v>
+        <v>790934</v>
+      </c>
+      <c r="E20" s="3" t="n">
+        <v>830050</v>
+      </c>
+      <c r="F20" s="3" t="n">
+        <v>829331</v>
+      </c>
+      <c r="G20" s="3" t="n">
+        <v>807536</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>Total Operating Expenses</t>
+          <t>Supplies</t>
         </is>
       </c>
       <c r="B21" s="3" t="n">
-        <v>154672</v>
+        <v>4015</v>
       </c>
       <c r="C21" s="3" t="n">
-        <v>143882</v>
+        <v>14593</v>
       </c>
       <c r="D21" s="3" t="n">
-        <v>71313</v>
+        <v>5620</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <v>5139</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <v>5683</v>
+      </c>
+      <c r="G21" s="3" t="n">
+        <v>9986</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>Income from Operations</t>
+          <t>Telephone, fax and internet</t>
         </is>
       </c>
       <c r="B22" s="3" t="n">
-        <v>331551</v>
+        <v>20534</v>
       </c>
       <c r="C22" s="3" t="n">
-        <v>213405</v>
+        <v>19428</v>
       </c>
       <c r="D22" s="3" t="n">
-        <v>219822</v>
+        <v>21250</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>22878</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>20761</v>
+      </c>
+      <c r="G22" s="3" t="n">
+        <v>21179</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>Earnings before Income Taxes</t>
-        </is>
-      </c>
-      <c r="B23" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C23" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="4" t="n">
-        <v>0</v>
+          <t>Travel</t>
+        </is>
+      </c>
+      <c r="B23" s="3" t="n">
+        <v>20661</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>23788</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>12847</v>
+      </c>
+      <c r="E23" s="3" t="n">
+        <v>16043</v>
+      </c>
+      <c r="F23" s="3" t="n">
+        <v>18135</v>
+      </c>
+      <c r="G23" s="3" t="n">
+        <v>23825</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>Income taxes</t>
+          <t>Utilities</t>
         </is>
       </c>
       <c r="B24" s="3" t="n">
-        <v>40449</v>
+        <v>21958</v>
       </c>
       <c r="C24" s="3" t="n">
-        <v>25286</v>
-      </c>
-      <c r="D24" s="4" t="n">
-        <v>0</v>
+        <v>20785</v>
+      </c>
+      <c r="D24" s="3" t="n">
+        <v>22831</v>
+      </c>
+      <c r="E24" s="3" t="n">
+        <v>23145</v>
+      </c>
+      <c r="F24" s="3" t="n">
+        <v>28957</v>
+      </c>
+      <c r="G24" s="3" t="n">
+        <v>25725</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>Net Income for the year</t>
+          <t>Vehicle</t>
         </is>
       </c>
       <c r="B25" s="3" t="n">
-        <v>291102</v>
+        <v>107249</v>
       </c>
       <c r="C25" s="3" t="n">
-        <v>188119</v>
+        <v>87354</v>
       </c>
       <c r="D25" s="3" t="n">
-        <v>220822</v>
+        <v>66091</v>
+      </c>
+      <c r="E25" s="3" t="n">
+        <v>66231</v>
+      </c>
+      <c r="F25" s="3" t="n">
+        <v>68912</v>
+      </c>
+      <c r="G25" s="3" t="n">
+        <v>73487</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>Normalizing Adjustments</t>
-        </is>
-      </c>
-      <c r="B26" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C26" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="4" t="n">
-        <v>0</v>
+          <t>Total Expenses</t>
+        </is>
+      </c>
+      <c r="B26" s="3" t="n">
+        <v>1580123</v>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>1535779</v>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>1372710</v>
+      </c>
+      <c r="E26" s="3" t="n">
+        <v>1398668</v>
+      </c>
+      <c r="F26" s="3" t="n">
+        <v>1409555</v>
+      </c>
+      <c r="G26" s="3" t="n">
+        <v>1443265</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Interest</t>
+          <t>Operating Income</t>
         </is>
       </c>
       <c r="B27" s="3" t="n">
-        <v>18300</v>
+        <v>251840</v>
       </c>
       <c r="C27" s="3" t="n">
-        <v>16776</v>
+        <v>276612</v>
       </c>
       <c r="D27" s="3" t="n">
-        <v>4093</v>
+        <v>235976</v>
+      </c>
+      <c r="E27" s="3" t="n">
+        <v>367475</v>
+      </c>
+      <c r="F27" s="3" t="n">
+        <v>227620</v>
+      </c>
+      <c r="G27" s="3" t="n">
+        <v>259242</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Income taxes</t>
-        </is>
-      </c>
-      <c r="B28" s="3" t="n">
-        <v>40449</v>
-      </c>
-      <c r="C28" s="3" t="n">
-        <v>25286</v>
+          <t>Other Income and (Expenses)</t>
+        </is>
+      </c>
+      <c r="B28" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="D28" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Donations</t>
-        </is>
-      </c>
-      <c r="B29" s="4" t="n">
-        <v>0</v>
+          <t>Gain (Loss) on asset disposal</t>
+        </is>
+      </c>
+      <c r="B29" s="3" t="n">
+        <v>31048</v>
       </c>
       <c r="C29" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D29" s="3" t="n">
-        <v>4000</v>
+      <c r="D29" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Salaries and wages</t>
+          <t>Foreign exchange gain (loss)</t>
         </is>
       </c>
       <c r="B30" s="4" t="n">
@@ -957,158 +1221,242 @@
         <v>0</v>
       </c>
       <c r="D30" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Cost of goods sold</t>
-        </is>
-      </c>
-      <c r="B31" s="3" t="n">
-        <v>44868</v>
-      </c>
-      <c r="C31" s="3" t="n">
-        <v>30217</v>
-      </c>
-      <c r="D31" s="3" t="n">
-        <v>12267</v>
+          <t>Other income</t>
+        </is>
+      </c>
+      <c r="B31" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Office expenses</t>
-        </is>
-      </c>
-      <c r="B32" s="3" t="n">
-        <v>19332</v>
-      </c>
-      <c r="C32" s="3" t="n">
-        <v>32748</v>
-      </c>
-      <c r="D32" s="3" t="n">
-        <v>17876</v>
+          <t>Total Other Income and (Expenses)</t>
+        </is>
+      </c>
+      <c r="B32" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="3" t="n">
+        <v>31048</v>
+      </c>
+      <c r="F32" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Meals and entertainment</t>
+          <t>EBITDA</t>
         </is>
       </c>
       <c r="B33" s="3" t="n">
-        <v>4657</v>
+        <v>251840</v>
       </c>
       <c r="C33" s="3" t="n">
-        <v>5830</v>
+        <v>276612</v>
       </c>
       <c r="D33" s="3" t="n">
-        <v>4619</v>
+        <v>235976</v>
+      </c>
+      <c r="E33" s="3" t="n">
+        <v>398523</v>
+      </c>
+      <c r="F33" s="3" t="n">
+        <v>227620</v>
+      </c>
+      <c r="G33" s="3" t="n">
+        <v>259242</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>Total Addbacks</t>
+          <t>Depreciation and Amortization</t>
         </is>
       </c>
       <c r="B34" s="3" t="n">
-        <v>189892</v>
+        <v>38161</v>
       </c>
       <c r="C34" s="3" t="n">
-        <v>155316</v>
+        <v>40437</v>
       </c>
       <c r="D34" s="3" t="n">
-        <v>41935</v>
+        <v>33625</v>
+      </c>
+      <c r="E34" s="3" t="n">
+        <v>14911</v>
+      </c>
+      <c r="F34" s="3" t="n">
+        <v>10426</v>
+      </c>
+      <c r="G34" s="3" t="n">
+        <v>8467</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Deductions</t>
-        </is>
-      </c>
-      <c r="B35" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C35" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D35" s="4" t="n">
-        <v>0</v>
+          <t>EBIT</t>
+        </is>
+      </c>
+      <c r="B35" s="3" t="n">
+        <v>213679</v>
+      </c>
+      <c r="C35" s="3" t="n">
+        <v>236175</v>
+      </c>
+      <c r="D35" s="3" t="n">
+        <v>202351</v>
+      </c>
+      <c r="E35" s="3" t="n">
+        <v>383612</v>
+      </c>
+      <c r="F35" s="3" t="n">
+        <v>217194</v>
+      </c>
+      <c r="G35" s="3" t="n">
+        <v>250775</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Owner salary replacement</t>
-        </is>
-      </c>
-      <c r="B36" s="3" t="n">
-        <v>-40000</v>
-      </c>
-      <c r="C36" s="3" t="n">
-        <v>-40000</v>
-      </c>
-      <c r="D36" s="3" t="n">
-        <v>-23333</v>
+          <t>Interest Expense</t>
+        </is>
+      </c>
+      <c r="B36" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>Total Deductions</t>
+          <t>EBT</t>
         </is>
       </c>
       <c r="B37" s="3" t="n">
-        <v>-40000</v>
+        <v>213679</v>
       </c>
       <c r="C37" s="3" t="n">
-        <v>-40000</v>
+        <v>236175</v>
       </c>
       <c r="D37" s="3" t="n">
-        <v>-23333</v>
+        <v>202351</v>
+      </c>
+      <c r="E37" s="3" t="n">
+        <v>383612</v>
+      </c>
+      <c r="F37" s="3" t="n">
+        <v>217194</v>
+      </c>
+      <c r="G37" s="3" t="n">
+        <v>250775</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>Normalized SDE</t>
-        </is>
-      </c>
-      <c r="B38" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C38" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" s="4" t="n">
-        <v>0</v>
+          <t>Provision for Income Taxes</t>
+        </is>
+      </c>
+      <c r="B38" s="3" t="n">
+        <v>29027</v>
+      </c>
+      <c r="C38" s="3" t="n">
+        <v>31171</v>
+      </c>
+      <c r="D38" s="3" t="n">
+        <v>25433</v>
+      </c>
+      <c r="E38" s="3" t="n">
+        <v>45943</v>
+      </c>
+      <c r="F38" s="3" t="n">
+        <v>27043</v>
+      </c>
+      <c r="G38" s="3" t="n">
+        <v>34451</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>SDE - 7 months</t>
-        </is>
-      </c>
-      <c r="B39" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C39" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="2" t="inlineStr"/>
-      <c r="B40" s="2" t="inlineStr"/>
-      <c r="C40" s="2" t="inlineStr"/>
-      <c r="D40" s="2" t="inlineStr"/>
+          <t>Net income (loss) after taxes</t>
+        </is>
+      </c>
+      <c r="B39" s="3" t="n">
+        <v>184652</v>
+      </c>
+      <c r="C39" s="3" t="n">
+        <v>205004</v>
+      </c>
+      <c r="D39" s="3" t="n">
+        <v>176918</v>
+      </c>
+      <c r="E39" s="3" t="n">
+        <v>337669</v>
+      </c>
+      <c r="F39" s="3" t="n">
+        <v>190151</v>
+      </c>
+      <c r="G39" s="3" t="n">
+        <v>216324</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>